<commit_message>
fix: deleting redundant folders
</commit_message>
<xml_diff>
--- a/SysCall-BackEnd/Tabela de Instâncias/Instancias - SysCall.xlsx
+++ b/SysCall-BackEnd/Tabela de Instâncias/Instancias - SysCall.xlsx
@@ -5,18 +5,17 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rsilva\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rsilva\Desktop\Syscall\SysCall-BackEnd\Tabela de Instâncias\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CD5ACE2D-07FF-44AD-AEBB-E3556ACC542E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{06A54C04-8300-45D4-A709-1CBA4A5B18D6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-2040" yWindow="-13620" windowWidth="24240" windowHeight="13020" xr2:uid="{B03A0472-E8DE-47A3-AA00-8C830A307724}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{B03A0472-E8DE-47A3-AA00-8C830A307724}"/>
   </bookViews>
   <sheets>
     <sheet name="Planilha1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -37,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="506" uniqueCount="208">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="474" uniqueCount="194">
   <si>
     <t>id</t>
   </si>
@@ -453,12 +452,6 @@
     <t>Lucas Silva</t>
   </si>
   <si>
-    <t>desbloqueado</t>
-  </si>
-  <si>
-    <t>Mariana Souza</t>
-  </si>
-  <si>
     <t>Felipe Oliveira</t>
   </si>
   <si>
@@ -471,75 +464,33 @@
     <t>Raphael Silva</t>
   </si>
   <si>
-    <t>Gustavo Rocha</t>
-  </si>
-  <si>
     <t>Fernanda Fernandes</t>
   </si>
   <si>
     <t>Patricia Gomes</t>
   </si>
   <si>
-    <t>bloqueado</t>
-  </si>
-  <si>
     <t>Juliana Almeida</t>
   </si>
   <si>
     <t>Rafael Carvalho</t>
   </si>
   <si>
-    <t>Beatriz Fernandes</t>
-  </si>
-  <si>
     <t>Debora Gomes</t>
   </si>
   <si>
-    <t>Enzo Martins</t>
-  </si>
-  <si>
-    <t>Camila Barbosa</t>
-  </si>
-  <si>
     <t>Helena Moura</t>
   </si>
   <si>
-    <t>Thiago Oliveira</t>
-  </si>
-  <si>
-    <t>Gabriel Ribeiro</t>
-  </si>
-  <si>
-    <t>Diego Ribeiro</t>
-  </si>
-  <si>
     <t>Beatriz Barbosa</t>
   </si>
   <si>
-    <t>Sandra Souza</t>
-  </si>
-  <si>
-    <t>Vanessa Pereira</t>
-  </si>
-  <si>
     <t>Marcio Costa</t>
   </si>
   <si>
-    <t>Larissa Freitas</t>
-  </si>
-  <si>
-    <t>Caio Rocha</t>
-  </si>
-  <si>
     <t>Victor Costa</t>
   </si>
   <si>
-    <t>Elaine Moura</t>
-  </si>
-  <si>
-    <t>Bruno Martins</t>
-  </si>
-  <si>
     <t>Aline Almeida</t>
   </si>
   <si>
@@ -558,9 +509,6 @@
     <t>R</t>
   </si>
   <si>
-    <t>schema_auth_recived_user</t>
-  </si>
-  <si>
     <t>schema_auth_requester_user</t>
   </si>
   <si>
@@ -645,22 +593,31 @@
     <t>TO</t>
   </si>
   <si>
-    <t>public.possible_location</t>
-  </si>
-  <si>
-    <t>auth.user</t>
-  </si>
-  <si>
     <t>public.contact</t>
   </si>
   <si>
-    <t>schema_public_location_id</t>
-  </si>
-  <si>
     <t>public.call_history</t>
   </si>
   <si>
     <t>user_id</t>
+  </si>
+  <si>
+    <t>U</t>
+  </si>
+  <si>
+    <t>B</t>
+  </si>
+  <si>
+    <t>possible_location</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        status</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        schema_auth_recived_user</t>
+  </si>
+  <si>
+    <t>public.user</t>
   </si>
 </sst>
 </file>
@@ -692,7 +649,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="8">
+  <fills count="9">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -732,6 +689,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFF99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.79998168889431442"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -778,7 +741,6 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -792,6 +754,9 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1141,10 +1106,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A1F702C4-BAA8-415A-A39B-B030BE0B18FC}">
-  <dimension ref="D3:K191"/>
+  <dimension ref="D36:K147"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="F33" sqref="F33"/>
+    <sheetView tabSelected="1" topLeftCell="A28" zoomScale="87" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="H34" sqref="H34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1154,243 +1119,13 @@
     <col min="6" max="6" width="22.42578125" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="19" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="36.28515625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="25.140625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="28.7109375" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="27" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="6:7" x14ac:dyDescent="0.25">
-      <c r="F3" s="11" t="s">
-        <v>202</v>
-      </c>
-      <c r="G3" s="11"/>
-    </row>
-    <row r="4" spans="6:7" x14ac:dyDescent="0.25">
-      <c r="F4" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="G4" s="2" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="5" spans="6:7" x14ac:dyDescent="0.25">
-      <c r="F5" s="7">
-        <v>1</v>
-      </c>
-      <c r="G5" s="3" t="s">
-        <v>175</v>
-      </c>
-    </row>
-    <row r="6" spans="6:7" x14ac:dyDescent="0.25">
-      <c r="F6" s="7">
-        <v>2</v>
-      </c>
-      <c r="G6" s="3" t="s">
-        <v>176</v>
-      </c>
-    </row>
-    <row r="7" spans="6:7" x14ac:dyDescent="0.25">
-      <c r="F7" s="7">
-        <v>3</v>
-      </c>
-      <c r="G7" s="3" t="s">
-        <v>177</v>
-      </c>
-    </row>
-    <row r="8" spans="6:7" x14ac:dyDescent="0.25">
-      <c r="F8" s="7">
-        <v>4</v>
-      </c>
-      <c r="G8" s="3" t="s">
-        <v>178</v>
-      </c>
-    </row>
-    <row r="9" spans="6:7" x14ac:dyDescent="0.25">
-      <c r="F9" s="7">
-        <v>5</v>
-      </c>
-      <c r="G9" s="3" t="s">
-        <v>179</v>
-      </c>
-    </row>
-    <row r="10" spans="6:7" x14ac:dyDescent="0.25">
-      <c r="F10" s="7">
-        <v>6</v>
-      </c>
-      <c r="G10" s="3" t="s">
-        <v>180</v>
-      </c>
-    </row>
-    <row r="11" spans="6:7" x14ac:dyDescent="0.25">
-      <c r="F11" s="7">
-        <v>7</v>
-      </c>
-      <c r="G11" s="3" t="s">
-        <v>181</v>
-      </c>
-    </row>
-    <row r="12" spans="6:7" x14ac:dyDescent="0.25">
-      <c r="F12" s="7">
-        <v>8</v>
-      </c>
-      <c r="G12" s="3" t="s">
-        <v>182</v>
-      </c>
-    </row>
-    <row r="13" spans="6:7" x14ac:dyDescent="0.25">
-      <c r="F13" s="7">
-        <v>9</v>
-      </c>
-      <c r="G13" s="3" t="s">
-        <v>183</v>
-      </c>
-    </row>
-    <row r="14" spans="6:7" x14ac:dyDescent="0.25">
-      <c r="F14" s="7">
-        <v>10</v>
-      </c>
-      <c r="G14" s="3" t="s">
-        <v>184</v>
-      </c>
-    </row>
-    <row r="15" spans="6:7" x14ac:dyDescent="0.25">
-      <c r="F15" s="7">
-        <v>11</v>
-      </c>
-      <c r="G15" s="3" t="s">
-        <v>185</v>
-      </c>
-    </row>
-    <row r="16" spans="6:7" x14ac:dyDescent="0.25">
-      <c r="F16" s="7">
-        <v>12</v>
-      </c>
-      <c r="G16" s="3" t="s">
-        <v>186</v>
-      </c>
-    </row>
-    <row r="17" spans="6:7" x14ac:dyDescent="0.25">
-      <c r="F17" s="7">
-        <v>13</v>
-      </c>
-      <c r="G17" s="3" t="s">
-        <v>187</v>
-      </c>
-    </row>
-    <row r="18" spans="6:7" x14ac:dyDescent="0.25">
-      <c r="F18" s="7">
-        <v>14</v>
-      </c>
-      <c r="G18" s="3" t="s">
-        <v>188</v>
-      </c>
-    </row>
-    <row r="19" spans="6:7" x14ac:dyDescent="0.25">
-      <c r="F19" s="7">
-        <v>15</v>
-      </c>
-      <c r="G19" s="3" t="s">
-        <v>189</v>
-      </c>
-    </row>
-    <row r="20" spans="6:7" x14ac:dyDescent="0.25">
-      <c r="F20" s="7">
-        <v>16</v>
-      </c>
-      <c r="G20" s="3" t="s">
-        <v>190</v>
-      </c>
-    </row>
-    <row r="21" spans="6:7" x14ac:dyDescent="0.25">
-      <c r="F21" s="7">
-        <v>17</v>
-      </c>
-      <c r="G21" s="3" t="s">
-        <v>191</v>
-      </c>
-    </row>
-    <row r="22" spans="6:7" x14ac:dyDescent="0.25">
-      <c r="F22" s="7">
-        <v>18</v>
-      </c>
-      <c r="G22" s="3" t="s">
-        <v>192</v>
-      </c>
-    </row>
-    <row r="23" spans="6:7" x14ac:dyDescent="0.25">
-      <c r="F23" s="7">
-        <v>19</v>
-      </c>
-      <c r="G23" s="3" t="s">
-        <v>193</v>
-      </c>
-    </row>
-    <row r="24" spans="6:7" x14ac:dyDescent="0.25">
-      <c r="F24" s="7">
-        <v>20</v>
-      </c>
-      <c r="G24" s="3" t="s">
-        <v>194</v>
-      </c>
-    </row>
-    <row r="25" spans="6:7" x14ac:dyDescent="0.25">
-      <c r="F25" s="7">
-        <v>21</v>
-      </c>
-      <c r="G25" s="3" t="s">
-        <v>195</v>
-      </c>
-    </row>
-    <row r="26" spans="6:7" x14ac:dyDescent="0.25">
-      <c r="F26" s="7">
-        <v>22</v>
-      </c>
-      <c r="G26" s="3" t="s">
-        <v>196</v>
-      </c>
-    </row>
-    <row r="27" spans="6:7" x14ac:dyDescent="0.25">
-      <c r="F27" s="7">
-        <v>23</v>
-      </c>
-      <c r="G27" s="3" t="s">
-        <v>197</v>
-      </c>
-    </row>
-    <row r="28" spans="6:7" x14ac:dyDescent="0.25">
-      <c r="F28" s="7">
-        <v>24</v>
-      </c>
-      <c r="G28" s="3" t="s">
-        <v>198</v>
-      </c>
-    </row>
-    <row r="29" spans="6:7" x14ac:dyDescent="0.25">
-      <c r="F29" s="7">
-        <v>25</v>
-      </c>
-      <c r="G29" s="3" t="s">
-        <v>199</v>
-      </c>
-    </row>
-    <row r="30" spans="6:7" x14ac:dyDescent="0.25">
-      <c r="F30" s="7">
-        <v>26</v>
-      </c>
-      <c r="G30" s="3" t="s">
-        <v>200</v>
-      </c>
-    </row>
-    <row r="31" spans="6:7" x14ac:dyDescent="0.25">
-      <c r="F31" s="7">
-        <v>27</v>
-      </c>
-      <c r="G31" s="3" t="s">
-        <v>201</v>
-      </c>
-    </row>
     <row r="36" spans="4:11" x14ac:dyDescent="0.25">
       <c r="D36" s="11" t="s">
-        <v>203</v>
+        <v>193</v>
       </c>
       <c r="E36" s="11"/>
       <c r="F36" s="11"/>
@@ -1402,7 +1137,7 @@
     </row>
     <row r="37" spans="4:11" x14ac:dyDescent="0.25">
       <c r="D37" s="1" t="s">
-        <v>207</v>
+        <v>187</v>
       </c>
       <c r="E37" s="1" t="s">
         <v>1</v>
@@ -1417,7 +1152,7 @@
         <v>4</v>
       </c>
       <c r="I37" s="1" t="s">
-        <v>205</v>
+        <v>190</v>
       </c>
       <c r="J37" s="1" t="s">
         <v>5</v>
@@ -1427,7 +1162,7 @@
       </c>
     </row>
     <row r="38" spans="4:11" x14ac:dyDescent="0.25">
-      <c r="D38" s="8">
+      <c r="D38" s="7">
         <v>1</v>
       </c>
       <c r="E38" s="3" t="s">
@@ -1442,8 +1177,8 @@
       <c r="H38" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="I38" s="7">
-        <v>25</v>
+      <c r="I38" s="6" t="s">
+        <v>182</v>
       </c>
       <c r="J38" s="3" t="s">
         <v>9</v>
@@ -1453,7 +1188,7 @@
       </c>
     </row>
     <row r="39" spans="4:11" x14ac:dyDescent="0.25">
-      <c r="D39" s="8">
+      <c r="D39" s="7">
         <v>2</v>
       </c>
       <c r="E39" s="3" t="s">
@@ -1468,8 +1203,8 @@
       <c r="H39" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="I39" s="7">
-        <v>25</v>
+      <c r="I39" s="6" t="s">
+        <v>182</v>
       </c>
       <c r="J39" s="3" t="s">
         <v>9</v>
@@ -1479,7 +1214,7 @@
       </c>
     </row>
     <row r="40" spans="4:11" x14ac:dyDescent="0.25">
-      <c r="D40" s="8">
+      <c r="D40" s="7">
         <v>3</v>
       </c>
       <c r="E40" s="3" t="s">
@@ -1494,8 +1229,8 @@
       <c r="H40" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="I40" s="7">
-        <v>25</v>
+      <c r="I40" s="6" t="s">
+        <v>182</v>
       </c>
       <c r="J40" s="3" t="s">
         <v>9</v>
@@ -1505,7 +1240,7 @@
       </c>
     </row>
     <row r="41" spans="4:11" x14ac:dyDescent="0.25">
-      <c r="D41" s="8">
+      <c r="D41" s="7">
         <v>4</v>
       </c>
       <c r="E41" s="3" t="s">
@@ -1520,8 +1255,8 @@
       <c r="H41" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="I41" s="7">
-        <v>25</v>
+      <c r="I41" s="6" t="s">
+        <v>182</v>
       </c>
       <c r="J41" s="3" t="s">
         <v>9</v>
@@ -1531,7 +1266,7 @@
       </c>
     </row>
     <row r="42" spans="4:11" x14ac:dyDescent="0.25">
-      <c r="D42" s="8">
+      <c r="D42" s="7">
         <v>5</v>
       </c>
       <c r="E42" s="3" t="s">
@@ -1546,8 +1281,8 @@
       <c r="H42" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="I42" s="7">
-        <v>25</v>
+      <c r="I42" s="6" t="s">
+        <v>182</v>
       </c>
       <c r="J42" s="3" t="s">
         <v>9</v>
@@ -1557,7 +1292,7 @@
       </c>
     </row>
     <row r="43" spans="4:11" x14ac:dyDescent="0.25">
-      <c r="D43" s="8">
+      <c r="D43" s="7">
         <v>6</v>
       </c>
       <c r="E43" s="3" t="s">
@@ -1572,8 +1307,8 @@
       <c r="H43" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="I43" s="7">
-        <v>25</v>
+      <c r="I43" s="6" t="s">
+        <v>182</v>
       </c>
       <c r="J43" s="3" t="s">
         <v>9</v>
@@ -1583,7 +1318,7 @@
       </c>
     </row>
     <row r="44" spans="4:11" x14ac:dyDescent="0.25">
-      <c r="D44" s="8">
+      <c r="D44" s="7">
         <v>7</v>
       </c>
       <c r="E44" s="3" t="s">
@@ -1598,8 +1333,8 @@
       <c r="H44" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="I44" s="7">
-        <v>25</v>
+      <c r="I44" s="6" t="s">
+        <v>182</v>
       </c>
       <c r="J44" s="3" t="s">
         <v>9</v>
@@ -1609,7 +1344,7 @@
       </c>
     </row>
     <row r="45" spans="4:11" x14ac:dyDescent="0.25">
-      <c r="D45" s="8">
+      <c r="D45" s="7">
         <v>8</v>
       </c>
       <c r="E45" s="3" t="s">
@@ -1624,8 +1359,8 @@
       <c r="H45" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="I45" s="7">
-        <v>25</v>
+      <c r="I45" s="6" t="s">
+        <v>182</v>
       </c>
       <c r="J45" s="3" t="s">
         <v>9</v>
@@ -1635,7 +1370,7 @@
       </c>
     </row>
     <row r="46" spans="4:11" x14ac:dyDescent="0.25">
-      <c r="D46" s="8">
+      <c r="D46" s="7">
         <v>9</v>
       </c>
       <c r="E46" s="3" t="s">
@@ -1650,8 +1385,8 @@
       <c r="H46" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="I46" s="7">
-        <v>25</v>
+      <c r="I46" s="6" t="s">
+        <v>182</v>
       </c>
       <c r="J46" s="3" t="s">
         <v>9</v>
@@ -1661,7 +1396,7 @@
       </c>
     </row>
     <row r="47" spans="4:11" x14ac:dyDescent="0.25">
-      <c r="D47" s="8">
+      <c r="D47" s="7">
         <v>10</v>
       </c>
       <c r="E47" s="3" t="s">
@@ -1676,8 +1411,8 @@
       <c r="H47" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="I47" s="7">
-        <v>25</v>
+      <c r="I47" s="6" t="s">
+        <v>182</v>
       </c>
       <c r="J47" s="3" t="s">
         <v>9</v>
@@ -1687,7 +1422,7 @@
       </c>
     </row>
     <row r="48" spans="4:11" x14ac:dyDescent="0.25">
-      <c r="D48" s="8">
+      <c r="D48" s="7">
         <v>11</v>
       </c>
       <c r="E48" s="3" t="s">
@@ -1702,8 +1437,8 @@
       <c r="H48" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="I48" s="7">
-        <v>19</v>
+      <c r="I48" s="6" t="s">
+        <v>176</v>
       </c>
       <c r="J48" s="3" t="s">
         <v>9</v>
@@ -1713,7 +1448,7 @@
       </c>
     </row>
     <row r="49" spans="4:11" x14ac:dyDescent="0.25">
-      <c r="D49" s="8">
+      <c r="D49" s="7">
         <v>12</v>
       </c>
       <c r="E49" s="3" t="s">
@@ -1728,8 +1463,8 @@
       <c r="H49" s="3" t="s">
         <v>42</v>
       </c>
-      <c r="I49" s="7">
-        <v>19</v>
+      <c r="I49" s="6" t="s">
+        <v>176</v>
       </c>
       <c r="J49" s="3" t="s">
         <v>9</v>
@@ -1739,7 +1474,7 @@
       </c>
     </row>
     <row r="50" spans="4:11" x14ac:dyDescent="0.25">
-      <c r="D50" s="8">
+      <c r="D50" s="7">
         <v>13</v>
       </c>
       <c r="E50" s="3" t="s">
@@ -1754,8 +1489,8 @@
       <c r="H50" s="3" t="s">
         <v>45</v>
       </c>
-      <c r="I50" s="7">
-        <v>19</v>
+      <c r="I50" s="6" t="s">
+        <v>176</v>
       </c>
       <c r="J50" s="3" t="s">
         <v>9</v>
@@ -1765,7 +1500,7 @@
       </c>
     </row>
     <row r="51" spans="4:11" x14ac:dyDescent="0.25">
-      <c r="D51" s="8">
+      <c r="D51" s="7">
         <v>14</v>
       </c>
       <c r="E51" s="3" t="s">
@@ -1780,8 +1515,8 @@
       <c r="H51" s="3" t="s">
         <v>48</v>
       </c>
-      <c r="I51" s="7">
-        <v>8</v>
+      <c r="I51" s="6" t="s">
+        <v>165</v>
       </c>
       <c r="J51" s="3" t="s">
         <v>9</v>
@@ -1791,7 +1526,7 @@
       </c>
     </row>
     <row r="52" spans="4:11" x14ac:dyDescent="0.25">
-      <c r="D52" s="8">
+      <c r="D52" s="7">
         <v>15</v>
       </c>
       <c r="E52" s="3" t="s">
@@ -1806,8 +1541,8 @@
       <c r="H52" s="3" t="s">
         <v>51</v>
       </c>
-      <c r="I52" s="7">
-        <v>8</v>
+      <c r="I52" s="6" t="s">
+        <v>165</v>
       </c>
       <c r="J52" s="3" t="s">
         <v>9</v>
@@ -1817,7 +1552,7 @@
       </c>
     </row>
     <row r="53" spans="4:11" x14ac:dyDescent="0.25">
-      <c r="D53" s="8">
+      <c r="D53" s="7">
         <v>16</v>
       </c>
       <c r="E53" s="3" t="s">
@@ -1832,8 +1567,8 @@
       <c r="H53" s="3" t="s">
         <v>54</v>
       </c>
-      <c r="I53" s="7">
-        <v>13</v>
+      <c r="I53" s="6" t="s">
+        <v>170</v>
       </c>
       <c r="J53" s="3" t="s">
         <v>9</v>
@@ -1843,7 +1578,7 @@
       </c>
     </row>
     <row r="54" spans="4:11" x14ac:dyDescent="0.25">
-      <c r="D54" s="8">
+      <c r="D54" s="7">
         <v>17</v>
       </c>
       <c r="E54" s="3" t="s">
@@ -1858,8 +1593,8 @@
       <c r="H54" s="3" t="s">
         <v>57</v>
       </c>
-      <c r="I54" s="7">
-        <v>13</v>
+      <c r="I54" s="6" t="s">
+        <v>170</v>
       </c>
       <c r="J54" s="3" t="s">
         <v>9</v>
@@ -1869,7 +1604,7 @@
       </c>
     </row>
     <row r="55" spans="4:11" x14ac:dyDescent="0.25">
-      <c r="D55" s="8">
+      <c r="D55" s="7">
         <v>18</v>
       </c>
       <c r="E55" s="3" t="s">
@@ -1884,8 +1619,8 @@
       <c r="H55" s="3" t="s">
         <v>60</v>
       </c>
-      <c r="I55" s="7">
-        <v>13</v>
+      <c r="I55" s="6" t="s">
+        <v>170</v>
       </c>
       <c r="J55" s="3" t="s">
         <v>9</v>
@@ -1895,7 +1630,7 @@
       </c>
     </row>
     <row r="56" spans="4:11" x14ac:dyDescent="0.25">
-      <c r="D56" s="8">
+      <c r="D56" s="7">
         <v>19</v>
       </c>
       <c r="E56" s="3" t="s">
@@ -1910,8 +1645,8 @@
       <c r="H56" s="3" t="s">
         <v>63</v>
       </c>
-      <c r="I56" s="7">
-        <v>13</v>
+      <c r="I56" s="6" t="s">
+        <v>170</v>
       </c>
       <c r="J56" s="3" t="s">
         <v>9</v>
@@ -1921,7 +1656,7 @@
       </c>
     </row>
     <row r="57" spans="4:11" x14ac:dyDescent="0.25">
-      <c r="D57" s="8">
+      <c r="D57" s="7">
         <v>20</v>
       </c>
       <c r="E57" s="3" t="s">
@@ -1936,8 +1671,8 @@
       <c r="H57" s="3" t="s">
         <v>65</v>
       </c>
-      <c r="I57" s="7">
-        <v>13</v>
+      <c r="I57" s="6" t="s">
+        <v>170</v>
       </c>
       <c r="J57" s="3" t="s">
         <v>9</v>
@@ -1947,7 +1682,7 @@
       </c>
     </row>
     <row r="58" spans="4:11" x14ac:dyDescent="0.25">
-      <c r="D58" s="8">
+      <c r="D58" s="7">
         <v>21</v>
       </c>
       <c r="E58" s="3" t="s">
@@ -1962,8 +1697,8 @@
       <c r="H58" s="3" t="s">
         <v>67</v>
       </c>
-      <c r="I58" s="7">
-        <v>13</v>
+      <c r="I58" s="6" t="s">
+        <v>170</v>
       </c>
       <c r="J58" s="3" t="s">
         <v>9</v>
@@ -1973,7 +1708,7 @@
       </c>
     </row>
     <row r="59" spans="4:11" x14ac:dyDescent="0.25">
-      <c r="D59" s="8">
+      <c r="D59" s="7">
         <v>22</v>
       </c>
       <c r="E59" s="3" t="s">
@@ -1988,8 +1723,8 @@
       <c r="H59" s="3" t="s">
         <v>69</v>
       </c>
-      <c r="I59" s="7">
-        <v>13</v>
+      <c r="I59" s="6" t="s">
+        <v>170</v>
       </c>
       <c r="J59" s="3" t="s">
         <v>9</v>
@@ -1999,7 +1734,7 @@
       </c>
     </row>
     <row r="60" spans="4:11" x14ac:dyDescent="0.25">
-      <c r="D60" s="8">
+      <c r="D60" s="7">
         <v>23</v>
       </c>
       <c r="E60" s="3" t="s">
@@ -2014,8 +1749,8 @@
       <c r="H60" s="3" t="s">
         <v>71</v>
       </c>
-      <c r="I60" s="7">
-        <v>16</v>
+      <c r="I60" s="6" t="s">
+        <v>173</v>
       </c>
       <c r="J60" s="3" t="s">
         <v>9</v>
@@ -2025,7 +1760,7 @@
       </c>
     </row>
     <row r="61" spans="4:11" x14ac:dyDescent="0.25">
-      <c r="D61" s="8">
+      <c r="D61" s="7">
         <v>24</v>
       </c>
       <c r="E61" s="3" t="s">
@@ -2040,8 +1775,8 @@
       <c r="H61" s="3" t="s">
         <v>73</v>
       </c>
-      <c r="I61" s="7">
-        <v>16</v>
+      <c r="I61" s="6" t="s">
+        <v>173</v>
       </c>
       <c r="J61" s="3" t="s">
         <v>9</v>
@@ -2051,7 +1786,7 @@
       </c>
     </row>
     <row r="62" spans="4:11" x14ac:dyDescent="0.25">
-      <c r="D62" s="8">
+      <c r="D62" s="7">
         <v>25</v>
       </c>
       <c r="E62" s="3" t="s">
@@ -2066,8 +1801,8 @@
       <c r="H62" s="3" t="s">
         <v>75</v>
       </c>
-      <c r="I62" s="7">
-        <v>16</v>
+      <c r="I62" s="6" t="s">
+        <v>173</v>
       </c>
       <c r="J62" s="3" t="s">
         <v>9</v>
@@ -2077,7 +1812,7 @@
       </c>
     </row>
     <row r="63" spans="4:11" x14ac:dyDescent="0.25">
-      <c r="D63" s="8">
+      <c r="D63" s="7">
         <v>26</v>
       </c>
       <c r="E63" s="3" t="s">
@@ -2092,8 +1827,8 @@
       <c r="H63" s="3" t="s">
         <v>77</v>
       </c>
-      <c r="I63" s="7">
-        <v>16</v>
+      <c r="I63" s="6" t="s">
+        <v>173</v>
       </c>
       <c r="J63" s="3" t="s">
         <v>9</v>
@@ -2103,7 +1838,7 @@
       </c>
     </row>
     <row r="64" spans="4:11" x14ac:dyDescent="0.25">
-      <c r="D64" s="8">
+      <c r="D64" s="7">
         <v>27</v>
       </c>
       <c r="E64" s="3" t="s">
@@ -2118,8 +1853,8 @@
       <c r="H64" s="3" t="s">
         <v>79</v>
       </c>
-      <c r="I64" s="7">
-        <v>16</v>
+      <c r="I64" s="6" t="s">
+        <v>173</v>
       </c>
       <c r="J64" s="3" t="s">
         <v>9</v>
@@ -2129,7 +1864,7 @@
       </c>
     </row>
     <row r="65" spans="4:11" x14ac:dyDescent="0.25">
-      <c r="D65" s="8">
+      <c r="D65" s="7">
         <v>28</v>
       </c>
       <c r="E65" s="3" t="s">
@@ -2144,8 +1879,8 @@
       <c r="H65" s="3" t="s">
         <v>81</v>
       </c>
-      <c r="I65" s="7">
-        <v>16</v>
+      <c r="I65" s="6" t="s">
+        <v>173</v>
       </c>
       <c r="J65" s="3" t="s">
         <v>9</v>
@@ -2155,7 +1890,7 @@
       </c>
     </row>
     <row r="66" spans="4:11" x14ac:dyDescent="0.25">
-      <c r="D66" s="8">
+      <c r="D66" s="7">
         <v>29</v>
       </c>
       <c r="E66" s="3" t="s">
@@ -2170,8 +1905,8 @@
       <c r="H66" s="3" t="s">
         <v>83</v>
       </c>
-      <c r="I66" s="7">
-        <v>24</v>
+      <c r="I66" s="6" t="s">
+        <v>181</v>
       </c>
       <c r="J66" s="3" t="s">
         <v>9</v>
@@ -2181,7 +1916,7 @@
       </c>
     </row>
     <row r="67" spans="4:11" x14ac:dyDescent="0.25">
-      <c r="D67" s="8">
+      <c r="D67" s="7">
         <v>30</v>
       </c>
       <c r="E67" s="3" t="s">
@@ -2196,8 +1931,8 @@
       <c r="H67" s="3" t="s">
         <v>85</v>
       </c>
-      <c r="I67" s="7">
-        <v>24</v>
+      <c r="I67" s="6" t="s">
+        <v>181</v>
       </c>
       <c r="J67" s="3" t="s">
         <v>9</v>
@@ -2207,7 +1942,7 @@
       </c>
     </row>
     <row r="68" spans="4:11" x14ac:dyDescent="0.25">
-      <c r="D68" s="8">
+      <c r="D68" s="7">
         <v>31</v>
       </c>
       <c r="E68" s="3" t="s">
@@ -2222,8 +1957,8 @@
       <c r="H68" s="3" t="s">
         <v>87</v>
       </c>
-      <c r="I68" s="7">
-        <v>24</v>
+      <c r="I68" s="6" t="s">
+        <v>181</v>
       </c>
       <c r="J68" s="3" t="s">
         <v>9</v>
@@ -2233,7 +1968,7 @@
       </c>
     </row>
     <row r="69" spans="4:11" x14ac:dyDescent="0.25">
-      <c r="D69" s="8">
+      <c r="D69" s="7">
         <v>32</v>
       </c>
       <c r="E69" s="3" t="s">
@@ -2248,8 +1983,8 @@
       <c r="H69" s="3" t="s">
         <v>89</v>
       </c>
-      <c r="I69" s="7">
-        <v>21</v>
+      <c r="I69" s="6" t="s">
+        <v>178</v>
       </c>
       <c r="J69" s="3" t="s">
         <v>9</v>
@@ -2259,7 +1994,7 @@
       </c>
     </row>
     <row r="70" spans="4:11" x14ac:dyDescent="0.25">
-      <c r="D70" s="8">
+      <c r="D70" s="7">
         <v>33</v>
       </c>
       <c r="E70" s="3" t="s">
@@ -2274,8 +2009,8 @@
       <c r="H70" s="3" t="s">
         <v>91</v>
       </c>
-      <c r="I70" s="7">
-        <v>21</v>
+      <c r="I70" s="6" t="s">
+        <v>178</v>
       </c>
       <c r="J70" s="3" t="s">
         <v>9</v>
@@ -2285,7 +2020,7 @@
       </c>
     </row>
     <row r="71" spans="4:11" x14ac:dyDescent="0.25">
-      <c r="D71" s="8">
+      <c r="D71" s="7">
         <v>34</v>
       </c>
       <c r="E71" s="3" t="s">
@@ -2300,8 +2035,8 @@
       <c r="H71" s="3" t="s">
         <v>93</v>
       </c>
-      <c r="I71" s="7">
-        <v>21</v>
+      <c r="I71" s="6" t="s">
+        <v>178</v>
       </c>
       <c r="J71" s="3" t="s">
         <v>9</v>
@@ -2311,7 +2046,7 @@
       </c>
     </row>
     <row r="72" spans="4:11" x14ac:dyDescent="0.25">
-      <c r="D72" s="8">
+      <c r="D72" s="7">
         <v>35</v>
       </c>
       <c r="E72" s="3" t="s">
@@ -2326,8 +2061,8 @@
       <c r="H72" s="3" t="s">
         <v>95</v>
       </c>
-      <c r="I72" s="7">
-        <v>21</v>
+      <c r="I72" s="6" t="s">
+        <v>178</v>
       </c>
       <c r="J72" s="3" t="s">
         <v>9</v>
@@ -2337,7 +2072,7 @@
       </c>
     </row>
     <row r="73" spans="4:11" x14ac:dyDescent="0.25">
-      <c r="D73" s="8">
+      <c r="D73" s="7">
         <v>36</v>
       </c>
       <c r="E73" s="3" t="s">
@@ -2352,8 +2087,8 @@
       <c r="H73" s="3" t="s">
         <v>97</v>
       </c>
-      <c r="I73" s="7">
-        <v>7</v>
+      <c r="I73" s="6" t="s">
+        <v>164</v>
       </c>
       <c r="J73" s="3" t="s">
         <v>9</v>
@@ -2363,7 +2098,7 @@
       </c>
     </row>
     <row r="74" spans="4:11" x14ac:dyDescent="0.25">
-      <c r="D74" s="8">
+      <c r="D74" s="7">
         <v>37</v>
       </c>
       <c r="E74" s="3" t="s">
@@ -2378,8 +2113,8 @@
       <c r="H74" s="3" t="s">
         <v>99</v>
       </c>
-      <c r="I74" s="7">
-        <v>9</v>
+      <c r="I74" s="6" t="s">
+        <v>166</v>
       </c>
       <c r="J74" s="3" t="s">
         <v>9</v>
@@ -2389,7 +2124,7 @@
       </c>
     </row>
     <row r="75" spans="4:11" x14ac:dyDescent="0.25">
-      <c r="D75" s="8">
+      <c r="D75" s="7">
         <v>38</v>
       </c>
       <c r="E75" s="3" t="s">
@@ -2404,8 +2139,8 @@
       <c r="H75" s="3" t="s">
         <v>101</v>
       </c>
-      <c r="I75" s="7">
-        <v>27</v>
+      <c r="I75" s="6" t="s">
+        <v>184</v>
       </c>
       <c r="J75" s="3" t="s">
         <v>9</v>
@@ -2415,7 +2150,7 @@
       </c>
     </row>
     <row r="76" spans="4:11" x14ac:dyDescent="0.25">
-      <c r="D76" s="8">
+      <c r="D76" s="7">
         <v>39</v>
       </c>
       <c r="E76" s="3" t="s">
@@ -2430,8 +2165,8 @@
       <c r="H76" s="3" t="s">
         <v>103</v>
       </c>
-      <c r="I76" s="7">
-        <v>9</v>
+      <c r="I76" s="6" t="s">
+        <v>166</v>
       </c>
       <c r="J76" s="3" t="s">
         <v>9</v>
@@ -2441,7 +2176,7 @@
       </c>
     </row>
     <row r="77" spans="4:11" x14ac:dyDescent="0.25">
-      <c r="D77" s="8">
+      <c r="D77" s="7">
         <v>40</v>
       </c>
       <c r="E77" s="3" t="s">
@@ -2456,8 +2191,8 @@
       <c r="H77" s="3" t="s">
         <v>105</v>
       </c>
-      <c r="I77" s="7">
-        <v>11</v>
+      <c r="I77" s="6" t="s">
+        <v>168</v>
       </c>
       <c r="J77" s="3" t="s">
         <v>9</v>
@@ -2467,7 +2202,7 @@
       </c>
     </row>
     <row r="78" spans="4:11" x14ac:dyDescent="0.25">
-      <c r="D78" s="8">
+      <c r="D78" s="7">
         <v>41</v>
       </c>
       <c r="E78" s="3" t="s">
@@ -2482,8 +2217,8 @@
       <c r="H78" s="3" t="s">
         <v>107</v>
       </c>
-      <c r="I78" s="7">
-        <v>11</v>
+      <c r="I78" s="6" t="s">
+        <v>168</v>
       </c>
       <c r="J78" s="3" t="s">
         <v>9</v>
@@ -2493,7 +2228,7 @@
       </c>
     </row>
     <row r="79" spans="4:11" x14ac:dyDescent="0.25">
-      <c r="D79" s="8">
+      <c r="D79" s="7">
         <v>42</v>
       </c>
       <c r="E79" s="3" t="s">
@@ -2508,8 +2243,8 @@
       <c r="H79" s="3" t="s">
         <v>108</v>
       </c>
-      <c r="I79" s="7">
-        <v>12</v>
+      <c r="I79" s="6" t="s">
+        <v>169</v>
       </c>
       <c r="J79" s="3" t="s">
         <v>9</v>
@@ -2519,7 +2254,7 @@
       </c>
     </row>
     <row r="80" spans="4:11" x14ac:dyDescent="0.25">
-      <c r="D80" s="8">
+      <c r="D80" s="7">
         <v>43</v>
       </c>
       <c r="E80" s="3" t="s">
@@ -2534,8 +2269,8 @@
       <c r="H80" s="3" t="s">
         <v>109</v>
       </c>
-      <c r="I80" s="7">
-        <v>1</v>
+      <c r="I80" s="6" t="s">
+        <v>158</v>
       </c>
       <c r="J80" s="3" t="s">
         <v>9</v>
@@ -2545,7 +2280,7 @@
       </c>
     </row>
     <row r="81" spans="4:11" x14ac:dyDescent="0.25">
-      <c r="D81" s="8">
+      <c r="D81" s="7">
         <v>44</v>
       </c>
       <c r="E81" s="3" t="s">
@@ -2560,8 +2295,8 @@
       <c r="H81" s="3" t="s">
         <v>110</v>
       </c>
-      <c r="I81" s="7">
-        <v>22</v>
+      <c r="I81" s="6" t="s">
+        <v>179</v>
       </c>
       <c r="J81" s="3" t="s">
         <v>9</v>
@@ -2571,7 +2306,7 @@
       </c>
     </row>
     <row r="82" spans="4:11" x14ac:dyDescent="0.25">
-      <c r="D82" s="8">
+      <c r="D82" s="7">
         <v>45</v>
       </c>
       <c r="E82" s="3" t="s">
@@ -2586,8 +2321,8 @@
       <c r="H82" s="3" t="s">
         <v>111</v>
       </c>
-      <c r="I82" s="7">
-        <v>5</v>
+      <c r="I82" s="6" t="s">
+        <v>162</v>
       </c>
       <c r="J82" s="3" t="s">
         <v>9</v>
@@ -2597,7 +2332,7 @@
       </c>
     </row>
     <row r="83" spans="4:11" x14ac:dyDescent="0.25">
-      <c r="D83" s="8">
+      <c r="D83" s="7">
         <v>46</v>
       </c>
       <c r="E83" s="3" t="s">
@@ -2612,8 +2347,8 @@
       <c r="H83" s="3" t="s">
         <v>112</v>
       </c>
-      <c r="I83" s="7">
-        <v>5</v>
+      <c r="I83" s="6" t="s">
+        <v>162</v>
       </c>
       <c r="J83" s="3" t="s">
         <v>9</v>
@@ -2623,7 +2358,7 @@
       </c>
     </row>
     <row r="84" spans="4:11" x14ac:dyDescent="0.25">
-      <c r="D84" s="8">
+      <c r="D84" s="7">
         <v>47</v>
       </c>
       <c r="E84" s="3" t="s">
@@ -2638,8 +2373,8 @@
       <c r="H84" s="3" t="s">
         <v>113</v>
       </c>
-      <c r="I84" s="7">
-        <v>5</v>
+      <c r="I84" s="6" t="s">
+        <v>162</v>
       </c>
       <c r="J84" s="3" t="s">
         <v>9</v>
@@ -2649,7 +2384,7 @@
       </c>
     </row>
     <row r="85" spans="4:11" x14ac:dyDescent="0.25">
-      <c r="D85" s="8">
+      <c r="D85" s="7">
         <v>48</v>
       </c>
       <c r="E85" s="3" t="s">
@@ -2664,8 +2399,8 @@
       <c r="H85" s="3" t="s">
         <v>114</v>
       </c>
-      <c r="I85" s="7">
-        <v>5</v>
+      <c r="I85" s="6" t="s">
+        <v>162</v>
       </c>
       <c r="J85" s="3" t="s">
         <v>9</v>
@@ -2675,7 +2410,7 @@
       </c>
     </row>
     <row r="86" spans="4:11" x14ac:dyDescent="0.25">
-      <c r="D86" s="8">
+      <c r="D86" s="7">
         <v>49</v>
       </c>
       <c r="E86" s="3" t="s">
@@ -2690,8 +2425,8 @@
       <c r="H86" s="3" t="s">
         <v>115</v>
       </c>
-      <c r="I86" s="7">
-        <v>5</v>
+      <c r="I86" s="6" t="s">
+        <v>162</v>
       </c>
       <c r="J86" s="3" t="s">
         <v>9</v>
@@ -2701,7 +2436,7 @@
       </c>
     </row>
     <row r="87" spans="4:11" x14ac:dyDescent="0.25">
-      <c r="D87" s="8">
+      <c r="D87" s="7">
         <v>50</v>
       </c>
       <c r="E87" s="3" t="s">
@@ -2716,8 +2451,8 @@
       <c r="H87" s="3" t="s">
         <v>116</v>
       </c>
-      <c r="I87" s="7">
-        <v>26</v>
+      <c r="I87" s="6" t="s">
+        <v>183</v>
       </c>
       <c r="J87" s="3" t="s">
         <v>9</v>
@@ -2727,7 +2462,7 @@
       </c>
     </row>
     <row r="88" spans="4:11" x14ac:dyDescent="0.25">
-      <c r="D88" s="8">
+      <c r="D88" s="7">
         <v>51</v>
       </c>
       <c r="E88" s="3" t="s">
@@ -2742,8 +2477,8 @@
       <c r="H88" s="3" t="s">
         <v>117</v>
       </c>
-      <c r="I88" s="7">
-        <v>17</v>
+      <c r="I88" s="6" t="s">
+        <v>174</v>
       </c>
       <c r="J88" s="3" t="s">
         <v>9</v>
@@ -2753,7 +2488,7 @@
       </c>
     </row>
     <row r="89" spans="4:11" x14ac:dyDescent="0.25">
-      <c r="D89" s="8">
+      <c r="D89" s="7">
         <v>52</v>
       </c>
       <c r="E89" s="3" t="s">
@@ -2768,8 +2503,8 @@
       <c r="H89" s="3" t="s">
         <v>118</v>
       </c>
-      <c r="I89" s="7">
-        <v>2</v>
+      <c r="I89" s="6" t="s">
+        <v>159</v>
       </c>
       <c r="J89" s="3" t="s">
         <v>9</v>
@@ -2779,7 +2514,7 @@
       </c>
     </row>
     <row r="90" spans="4:11" x14ac:dyDescent="0.25">
-      <c r="D90" s="8">
+      <c r="D90" s="7">
         <v>53</v>
       </c>
       <c r="E90" s="3" t="s">
@@ -2794,8 +2529,8 @@
       <c r="H90" s="3" t="s">
         <v>119</v>
       </c>
-      <c r="I90" s="7">
-        <v>15</v>
+      <c r="I90" s="6" t="s">
+        <v>172</v>
       </c>
       <c r="J90" s="3" t="s">
         <v>9</v>
@@ -2805,7 +2540,7 @@
       </c>
     </row>
     <row r="91" spans="4:11" x14ac:dyDescent="0.25">
-      <c r="D91" s="8">
+      <c r="D91" s="7">
         <v>54</v>
       </c>
       <c r="E91" s="3" t="s">
@@ -2820,8 +2555,8 @@
       <c r="H91" s="3" t="s">
         <v>120</v>
       </c>
-      <c r="I91" s="7">
-        <v>20</v>
+      <c r="I91" s="6" t="s">
+        <v>177</v>
       </c>
       <c r="J91" s="3" t="s">
         <v>9</v>
@@ -2831,7 +2566,7 @@
       </c>
     </row>
     <row r="92" spans="4:11" x14ac:dyDescent="0.25">
-      <c r="D92" s="8">
+      <c r="D92" s="7">
         <v>55</v>
       </c>
       <c r="E92" s="3" t="s">
@@ -2846,8 +2581,8 @@
       <c r="H92" s="3" t="s">
         <v>121</v>
       </c>
-      <c r="I92" s="7">
-        <v>6</v>
+      <c r="I92" s="6" t="s">
+        <v>163</v>
       </c>
       <c r="J92" s="3" t="s">
         <v>9</v>
@@ -2857,7 +2592,7 @@
       </c>
     </row>
     <row r="93" spans="4:11" x14ac:dyDescent="0.25">
-      <c r="D93" s="8">
+      <c r="D93" s="7">
         <v>56</v>
       </c>
       <c r="E93" s="3" t="s">
@@ -2872,8 +2607,8 @@
       <c r="H93" s="3" t="s">
         <v>122</v>
       </c>
-      <c r="I93" s="7">
-        <v>18</v>
+      <c r="I93" s="6" t="s">
+        <v>175</v>
       </c>
       <c r="J93" s="3" t="s">
         <v>9</v>
@@ -2883,7 +2618,7 @@
       </c>
     </row>
     <row r="94" spans="4:11" x14ac:dyDescent="0.25">
-      <c r="D94" s="8">
+      <c r="D94" s="7">
         <v>57</v>
       </c>
       <c r="E94" s="3" t="s">
@@ -2898,8 +2633,8 @@
       <c r="H94" s="3" t="s">
         <v>123</v>
       </c>
-      <c r="I94" s="7">
-        <v>17</v>
+      <c r="I94" s="6" t="s">
+        <v>174</v>
       </c>
       <c r="J94" s="3" t="s">
         <v>9</v>
@@ -2909,7 +2644,7 @@
       </c>
     </row>
     <row r="95" spans="4:11" x14ac:dyDescent="0.25">
-      <c r="D95" s="8">
+      <c r="D95" s="7">
         <v>58</v>
       </c>
       <c r="E95" s="3" t="s">
@@ -2924,8 +2659,8 @@
       <c r="H95" s="3" t="s">
         <v>124</v>
       </c>
-      <c r="I95" s="7">
-        <v>6</v>
+      <c r="I95" s="6" t="s">
+        <v>163</v>
       </c>
       <c r="J95" s="3" t="s">
         <v>9</v>
@@ -2935,7 +2670,7 @@
       </c>
     </row>
     <row r="96" spans="4:11" x14ac:dyDescent="0.25">
-      <c r="D96" s="8">
+      <c r="D96" s="7">
         <v>59</v>
       </c>
       <c r="E96" s="3" t="s">
@@ -2950,8 +2685,8 @@
       <c r="H96" s="3" t="s">
         <v>125</v>
       </c>
-      <c r="I96" s="7">
-        <v>18</v>
+      <c r="I96" s="6" t="s">
+        <v>175</v>
       </c>
       <c r="J96" s="3" t="s">
         <v>9</v>
@@ -2961,7 +2696,7 @@
       </c>
     </row>
     <row r="97" spans="4:11" x14ac:dyDescent="0.25">
-      <c r="D97" s="8">
+      <c r="D97" s="7">
         <v>60</v>
       </c>
       <c r="E97" s="3" t="s">
@@ -2976,8 +2711,8 @@
       <c r="H97" s="3" t="s">
         <v>126</v>
       </c>
-      <c r="I97" s="7">
-        <v>14</v>
+      <c r="I97" s="6" t="s">
+        <v>171</v>
       </c>
       <c r="J97" s="3" t="s">
         <v>9</v>
@@ -2987,7 +2722,7 @@
       </c>
     </row>
     <row r="98" spans="4:11" x14ac:dyDescent="0.25">
-      <c r="D98" s="8">
+      <c r="D98" s="7">
         <v>61</v>
       </c>
       <c r="E98" s="3" t="s">
@@ -3002,8 +2737,8 @@
       <c r="H98" s="3" t="s">
         <v>127</v>
       </c>
-      <c r="I98" s="7">
-        <v>4</v>
+      <c r="I98" s="6" t="s">
+        <v>161</v>
       </c>
       <c r="J98" s="3" t="s">
         <v>9</v>
@@ -3013,7 +2748,7 @@
       </c>
     </row>
     <row r="99" spans="4:11" x14ac:dyDescent="0.25">
-      <c r="D99" s="8">
+      <c r="D99" s="7">
         <v>62</v>
       </c>
       <c r="E99" s="3" t="s">
@@ -3028,8 +2763,8 @@
       <c r="H99" s="3" t="s">
         <v>128</v>
       </c>
-      <c r="I99" s="7">
-        <v>14</v>
+      <c r="I99" s="6" t="s">
+        <v>171</v>
       </c>
       <c r="J99" s="3" t="s">
         <v>9</v>
@@ -3039,7 +2774,7 @@
       </c>
     </row>
     <row r="100" spans="4:11" x14ac:dyDescent="0.25">
-      <c r="D100" s="8">
+      <c r="D100" s="7">
         <v>63</v>
       </c>
       <c r="E100" s="3" t="s">
@@ -3054,8 +2789,8 @@
       <c r="H100" s="3" t="s">
         <v>129</v>
       </c>
-      <c r="I100" s="7">
-        <v>14</v>
+      <c r="I100" s="6" t="s">
+        <v>171</v>
       </c>
       <c r="J100" s="3" t="s">
         <v>9</v>
@@ -3065,7 +2800,7 @@
       </c>
     </row>
     <row r="101" spans="4:11" x14ac:dyDescent="0.25">
-      <c r="D101" s="8">
+      <c r="D101" s="7">
         <v>64</v>
       </c>
       <c r="E101" s="3" t="s">
@@ -3080,8 +2815,8 @@
       <c r="H101" s="3" t="s">
         <v>130</v>
       </c>
-      <c r="I101" s="7">
-        <v>23</v>
+      <c r="I101" s="6" t="s">
+        <v>180</v>
       </c>
       <c r="J101" s="3" t="s">
         <v>9</v>
@@ -3091,7 +2826,7 @@
       </c>
     </row>
     <row r="102" spans="4:11" x14ac:dyDescent="0.25">
-      <c r="D102" s="8">
+      <c r="D102" s="7">
         <v>65</v>
       </c>
       <c r="E102" s="3" t="s">
@@ -3106,8 +2841,8 @@
       <c r="H102" s="3" t="s">
         <v>131</v>
       </c>
-      <c r="I102" s="7">
-        <v>3</v>
+      <c r="I102" s="6" t="s">
+        <v>160</v>
       </c>
       <c r="J102" s="3" t="s">
         <v>9</v>
@@ -3117,7 +2852,7 @@
       </c>
     </row>
     <row r="103" spans="4:11" x14ac:dyDescent="0.25">
-      <c r="D103" s="8">
+      <c r="D103" s="7">
         <v>66</v>
       </c>
       <c r="E103" s="3" t="s">
@@ -3132,8 +2867,8 @@
       <c r="H103" s="3" t="s">
         <v>132</v>
       </c>
-      <c r="I103" s="7">
-        <v>4</v>
+      <c r="I103" s="6" t="s">
+        <v>161</v>
       </c>
       <c r="J103" s="3" t="s">
         <v>9</v>
@@ -3143,7 +2878,7 @@
       </c>
     </row>
     <row r="104" spans="4:11" x14ac:dyDescent="0.25">
-      <c r="D104" s="8">
+      <c r="D104" s="7">
         <v>67</v>
       </c>
       <c r="E104" s="3" t="s">
@@ -3158,8 +2893,8 @@
       <c r="H104" s="3" t="s">
         <v>133</v>
       </c>
-      <c r="I104" s="7">
-        <v>10</v>
+      <c r="I104" s="6" t="s">
+        <v>167</v>
       </c>
       <c r="J104" s="3" t="s">
         <v>9</v>
@@ -3169,7 +2904,7 @@
       </c>
     </row>
     <row r="105" spans="4:11" x14ac:dyDescent="0.25">
-      <c r="D105" s="8">
+      <c r="D105" s="7">
         <v>68</v>
       </c>
       <c r="E105" s="3" t="s">
@@ -3184,8 +2919,8 @@
       <c r="H105" s="3" t="s">
         <v>134</v>
       </c>
-      <c r="I105" s="7">
-        <v>10</v>
+      <c r="I105" s="6" t="s">
+        <v>167</v>
       </c>
       <c r="J105" s="3" t="s">
         <v>9</v>
@@ -3196,7 +2931,7 @@
     </row>
     <row r="110" spans="4:11" x14ac:dyDescent="0.25">
       <c r="F110" s="11" t="s">
-        <v>204</v>
+        <v>185</v>
       </c>
       <c r="G110" s="11"/>
       <c r="H110" s="11"/>
@@ -3204,1327 +2939,561 @@
       <c r="J110" s="11"/>
     </row>
     <row r="111" spans="4:11" x14ac:dyDescent="0.25">
-      <c r="F111" s="2" t="s">
+      <c r="F111" s="10" t="s">
         <v>0</v>
       </c>
-      <c r="G111" s="5" t="s">
+      <c r="G111" s="10" t="s">
         <v>135</v>
       </c>
-      <c r="H111" s="5" t="s">
+      <c r="H111" s="10" t="s">
+        <v>191</v>
+      </c>
+      <c r="I111" s="10" t="s">
+        <v>153</v>
+      </c>
+      <c r="J111" s="10" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="112" spans="4:11" x14ac:dyDescent="0.25">
+      <c r="F112" s="8">
+        <v>1</v>
+      </c>
+      <c r="G112" s="3" t="s">
+        <v>140</v>
+      </c>
+      <c r="H112" s="3" t="s">
+        <v>188</v>
+      </c>
+      <c r="I112" s="7">
+        <v>6</v>
+      </c>
+      <c r="J112" s="7">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="113" spans="6:10" x14ac:dyDescent="0.25">
+      <c r="F113" s="8">
+        <v>2</v>
+      </c>
+      <c r="G113" s="3" t="s">
+        <v>146</v>
+      </c>
+      <c r="H113" s="3" t="s">
+        <v>188</v>
+      </c>
+      <c r="I113" s="7">
+        <v>29</v>
+      </c>
+      <c r="J113" s="7">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="114" spans="6:10" x14ac:dyDescent="0.25">
+      <c r="F114" s="8">
+        <v>3</v>
+      </c>
+      <c r="G114" s="3" t="s">
+        <v>143</v>
+      </c>
+      <c r="H114" s="3" t="s">
+        <v>189</v>
+      </c>
+      <c r="I114" s="7">
+        <v>11</v>
+      </c>
+      <c r="J114" s="7">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="115" spans="6:10" x14ac:dyDescent="0.25">
+      <c r="F115" s="8">
+        <v>4</v>
+      </c>
+      <c r="G115" s="3" t="s">
+        <v>144</v>
+      </c>
+      <c r="H115" s="3" t="s">
+        <v>188</v>
+      </c>
+      <c r="I115" s="7">
+        <v>7</v>
+      </c>
+      <c r="J115" s="7">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="116" spans="6:10" x14ac:dyDescent="0.25">
+      <c r="F116" s="8">
+        <v>5</v>
+      </c>
+      <c r="G116" s="3" t="s">
+        <v>139</v>
+      </c>
+      <c r="H116" s="3" t="s">
+        <v>188</v>
+      </c>
+      <c r="I116" s="7">
+        <v>5</v>
+      </c>
+      <c r="J116" s="7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="117" spans="6:10" x14ac:dyDescent="0.25">
+      <c r="F117" s="8">
+        <v>6</v>
+      </c>
+      <c r="G117" s="3" t="s">
+        <v>137</v>
+      </c>
+      <c r="H117" s="3" t="s">
+        <v>188</v>
+      </c>
+      <c r="I117" s="7">
+        <v>2</v>
+      </c>
+      <c r="J117" s="7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="118" spans="6:10" x14ac:dyDescent="0.25">
+      <c r="F118" s="8">
+        <v>7</v>
+      </c>
+      <c r="G118" s="3" t="s">
+        <v>145</v>
+      </c>
+      <c r="H118" s="3" t="s">
+        <v>188</v>
+      </c>
+      <c r="I118" s="7">
+        <v>10</v>
+      </c>
+      <c r="J118" s="7">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="119" spans="6:10" x14ac:dyDescent="0.25">
+      <c r="F119" s="8">
+        <v>8</v>
+      </c>
+      <c r="G119" s="3" t="s">
+        <v>148</v>
+      </c>
+      <c r="H119" s="3" t="s">
+        <v>188</v>
+      </c>
+      <c r="I119" s="7">
+        <v>49</v>
+      </c>
+      <c r="J119" s="7">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="120" spans="6:10" x14ac:dyDescent="0.25">
+      <c r="F120" s="8">
+        <v>9</v>
+      </c>
+      <c r="G120" s="3" t="s">
+        <v>150</v>
+      </c>
+      <c r="H120" s="3" t="s">
+        <v>188</v>
+      </c>
+      <c r="I120" s="7">
+        <v>24</v>
+      </c>
+      <c r="J120" s="7">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="121" spans="6:10" x14ac:dyDescent="0.25">
+      <c r="F121" s="8">
+        <v>10</v>
+      </c>
+      <c r="G121" s="3" t="s">
+        <v>142</v>
+      </c>
+      <c r="H121" s="3" t="s">
+        <v>188</v>
+      </c>
+      <c r="I121" s="7">
+        <v>9</v>
+      </c>
+      <c r="J121" s="7">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="122" spans="6:10" x14ac:dyDescent="0.25">
+      <c r="F122" s="8">
+        <v>11</v>
+      </c>
+      <c r="G122" s="3" t="s">
+        <v>149</v>
+      </c>
+      <c r="H122" s="3" t="s">
+        <v>188</v>
+      </c>
+      <c r="I122" s="7">
+        <v>60</v>
+      </c>
+      <c r="J122" s="7">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="123" spans="6:10" x14ac:dyDescent="0.25">
+      <c r="F123" s="8">
+        <v>12</v>
+      </c>
+      <c r="G123" s="3" t="s">
+        <v>138</v>
+      </c>
+      <c r="H123" s="3" t="s">
+        <v>188</v>
+      </c>
+      <c r="I123" s="7">
+        <v>4</v>
+      </c>
+      <c r="J123" s="7">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="124" spans="6:10" x14ac:dyDescent="0.25">
+      <c r="F124" s="8">
+        <v>13</v>
+      </c>
+      <c r="G124" s="3" t="s">
+        <v>147</v>
+      </c>
+      <c r="H124" s="3" t="s">
+        <v>189</v>
+      </c>
+      <c r="I124" s="7">
+        <v>33</v>
+      </c>
+      <c r="J124" s="7">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="125" spans="6:10" x14ac:dyDescent="0.25">
+      <c r="F125" s="8">
+        <v>14</v>
+      </c>
+      <c r="G125" s="3" t="s">
+        <v>141</v>
+      </c>
+      <c r="H125" s="3" t="s">
+        <v>189</v>
+      </c>
+      <c r="I125" s="7">
+        <v>1</v>
+      </c>
+      <c r="J125" s="7">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="126" spans="6:10" x14ac:dyDescent="0.25">
+      <c r="F126" s="8">
+        <v>15</v>
+      </c>
+      <c r="G126" s="3" t="s">
+        <v>151</v>
+      </c>
+      <c r="H126" s="3" t="s">
+        <v>188</v>
+      </c>
+      <c r="I126" s="7">
+        <v>25</v>
+      </c>
+      <c r="J126" s="7">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="131" spans="6:10" x14ac:dyDescent="0.25">
+      <c r="F131" s="11" t="s">
+        <v>186</v>
+      </c>
+      <c r="G131" s="11"/>
+      <c r="H131" s="11"/>
+      <c r="I131" s="11"/>
+      <c r="J131" s="11"/>
+    </row>
+    <row r="132" spans="6:10" x14ac:dyDescent="0.25">
+      <c r="F132" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="G132" s="2" t="s">
         <v>136</v>
       </c>
-      <c r="I111" s="5" t="s">
-        <v>169</v>
-      </c>
-      <c r="J111" s="5" t="s">
-        <v>170</v>
-      </c>
-    </row>
-    <row r="112" spans="4:11" x14ac:dyDescent="0.25">
-      <c r="F112" s="9">
-        <v>1</v>
-      </c>
-      <c r="G112" s="3" t="s">
-        <v>142</v>
-      </c>
-      <c r="H112" s="3" t="s">
-        <v>138</v>
-      </c>
-      <c r="I112" s="8">
-        <v>6</v>
-      </c>
-      <c r="J112" s="8">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="113" spans="6:10" x14ac:dyDescent="0.25">
-      <c r="F113" s="9">
-        <v>2</v>
-      </c>
-      <c r="G113" s="3" t="s">
-        <v>151</v>
-      </c>
-      <c r="H113" s="3" t="s">
-        <v>138</v>
-      </c>
-      <c r="I113" s="8">
-        <v>29</v>
-      </c>
-      <c r="J113" s="8">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="114" spans="6:10" x14ac:dyDescent="0.25">
-      <c r="F114" s="9">
-        <v>3</v>
-      </c>
-      <c r="G114" s="3" t="s">
-        <v>146</v>
-      </c>
-      <c r="H114" s="3" t="s">
-        <v>147</v>
-      </c>
-      <c r="I114" s="8">
-        <v>11</v>
-      </c>
-      <c r="J114" s="8">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="115" spans="6:10" x14ac:dyDescent="0.25">
-      <c r="F115" s="9">
-        <v>4</v>
-      </c>
-      <c r="G115" s="3" t="s">
-        <v>148</v>
-      </c>
-      <c r="H115" s="3" t="s">
-        <v>138</v>
-      </c>
-      <c r="I115" s="8">
-        <v>7</v>
-      </c>
-      <c r="J115" s="8">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="116" spans="6:10" x14ac:dyDescent="0.25">
-      <c r="F116" s="9">
-        <v>5</v>
-      </c>
-      <c r="G116" s="3" t="s">
-        <v>162</v>
-      </c>
-      <c r="H116" s="3" t="s">
-        <v>138</v>
-      </c>
-      <c r="I116" s="8">
-        <v>17</v>
-      </c>
-      <c r="J116" s="8">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="117" spans="6:10" x14ac:dyDescent="0.25">
-      <c r="F117" s="9">
-        <v>6</v>
-      </c>
-      <c r="G117" s="3" t="s">
-        <v>141</v>
-      </c>
-      <c r="H117" s="3" t="s">
-        <v>138</v>
-      </c>
-      <c r="I117" s="8">
-        <v>5</v>
-      </c>
-      <c r="J117" s="8">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="118" spans="6:10" x14ac:dyDescent="0.25">
-      <c r="F118" s="9">
-        <v>7</v>
-      </c>
-      <c r="G118" s="3" t="s">
-        <v>137</v>
-      </c>
-      <c r="H118" s="3" t="s">
-        <v>138</v>
-      </c>
-      <c r="I118" s="8">
-        <v>2</v>
-      </c>
-      <c r="J118" s="8">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="119" spans="6:10" x14ac:dyDescent="0.25">
-      <c r="F119" s="9">
-        <v>8</v>
-      </c>
-      <c r="G119" s="3" t="s">
-        <v>163</v>
-      </c>
-      <c r="H119" s="3" t="s">
-        <v>138</v>
-      </c>
-      <c r="I119" s="8">
-        <v>28</v>
-      </c>
-      <c r="J119" s="8">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="120" spans="6:10" x14ac:dyDescent="0.25">
-      <c r="F120" s="9">
-        <v>9</v>
-      </c>
-      <c r="G120" s="3" t="s">
-        <v>149</v>
-      </c>
-      <c r="H120" s="3" t="s">
-        <v>138</v>
-      </c>
-      <c r="I120" s="8">
-        <v>10</v>
-      </c>
-      <c r="J120" s="8">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="121" spans="6:10" x14ac:dyDescent="0.25">
-      <c r="F121" s="9">
-        <v>10</v>
-      </c>
-      <c r="G121" s="3" t="s">
+      <c r="H132" s="2" t="s">
         <v>152</v>
       </c>
-      <c r="H121" s="3" t="s">
-        <v>138</v>
-      </c>
-      <c r="I121" s="8">
-        <v>30</v>
-      </c>
-      <c r="J121" s="8">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="122" spans="6:10" x14ac:dyDescent="0.25">
-      <c r="F122" s="9">
-        <v>11</v>
-      </c>
-      <c r="G122" s="3" t="s">
-        <v>161</v>
-      </c>
-      <c r="H122" s="3" t="s">
-        <v>138</v>
-      </c>
-      <c r="I122" s="8">
-        <v>60</v>
-      </c>
-      <c r="J122" s="8">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="123" spans="6:10" x14ac:dyDescent="0.25">
-      <c r="F123" s="9">
-        <v>12</v>
-      </c>
-      <c r="G123" s="3" t="s">
-        <v>158</v>
-      </c>
-      <c r="H123" s="3" t="s">
-        <v>138</v>
-      </c>
-      <c r="I123" s="8">
-        <v>49</v>
-      </c>
-      <c r="J123" s="8">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="124" spans="6:10" x14ac:dyDescent="0.25">
-      <c r="F124" s="9">
-        <v>13</v>
-      </c>
-      <c r="G124" s="3" t="s">
-        <v>150</v>
-      </c>
-      <c r="H124" s="3" t="s">
-        <v>138</v>
-      </c>
-      <c r="I124" s="8">
-        <v>27</v>
-      </c>
-      <c r="J124" s="8">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="125" spans="6:10" x14ac:dyDescent="0.25">
-      <c r="F125" s="9">
-        <v>14</v>
-      </c>
-      <c r="G125" s="3" t="s">
-        <v>144</v>
-      </c>
-      <c r="H125" s="3" t="s">
-        <v>138</v>
-      </c>
-      <c r="I125" s="8">
-        <v>8</v>
-      </c>
-      <c r="J125" s="8">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="126" spans="6:10" x14ac:dyDescent="0.25">
-      <c r="F126" s="9">
-        <v>15</v>
-      </c>
-      <c r="G126" s="3" t="s">
-        <v>164</v>
-      </c>
-      <c r="H126" s="3" t="s">
-        <v>138</v>
-      </c>
-      <c r="I126" s="8">
-        <v>24</v>
-      </c>
-      <c r="J126" s="8">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="127" spans="6:10" x14ac:dyDescent="0.25">
-      <c r="F127" s="9">
-        <v>16</v>
-      </c>
-      <c r="G127" s="3" t="s">
-        <v>145</v>
-      </c>
-      <c r="H127" s="3" t="s">
-        <v>138</v>
-      </c>
-      <c r="I127" s="8">
-        <v>9</v>
-      </c>
-      <c r="J127" s="8">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="128" spans="6:10" x14ac:dyDescent="0.25">
-      <c r="F128" s="9">
-        <v>17</v>
-      </c>
-      <c r="G128" s="3" t="s">
-        <v>153</v>
-      </c>
-      <c r="H128" s="3" t="s">
-        <v>138</v>
-      </c>
-      <c r="I128" s="8">
-        <v>13</v>
-      </c>
-      <c r="J128" s="8">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="129" spans="6:10" x14ac:dyDescent="0.25">
-      <c r="F129" s="9">
-        <v>18</v>
-      </c>
-      <c r="G129" s="3" t="s">
-        <v>159</v>
-      </c>
-      <c r="H129" s="3" t="s">
-        <v>138</v>
-      </c>
-      <c r="I129" s="8">
-        <v>21</v>
-      </c>
-      <c r="J129" s="8">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="130" spans="6:10" x14ac:dyDescent="0.25">
-      <c r="F130" s="9">
-        <v>19</v>
-      </c>
-      <c r="G130" s="3" t="s">
-        <v>155</v>
-      </c>
-      <c r="H130" s="3" t="s">
-        <v>138</v>
-      </c>
-      <c r="I130" s="8">
-        <v>22</v>
-      </c>
-      <c r="J130" s="8">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="131" spans="6:10" x14ac:dyDescent="0.25">
-      <c r="F131" s="9">
-        <v>20</v>
-      </c>
-      <c r="G131" s="3" t="s">
-        <v>165</v>
-      </c>
-      <c r="H131" s="3" t="s">
-        <v>138</v>
-      </c>
-      <c r="I131" s="8">
-        <v>15</v>
-      </c>
-      <c r="J131" s="8">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="132" spans="6:10" x14ac:dyDescent="0.25">
-      <c r="F132" s="9">
-        <v>21</v>
-      </c>
-      <c r="G132" s="3" t="s">
-        <v>140</v>
-      </c>
-      <c r="H132" s="3" t="s">
-        <v>138</v>
-      </c>
-      <c r="I132" s="8">
-        <v>4</v>
-      </c>
-      <c r="J132" s="8">
-        <v>6</v>
+      <c r="I132" s="2" t="s">
+        <v>192</v>
+      </c>
+      <c r="J132" s="2" t="s">
+        <v>157</v>
       </c>
     </row>
     <row r="133" spans="6:10" x14ac:dyDescent="0.25">
       <c r="F133" s="9">
-        <v>22</v>
+        <v>1</v>
       </c>
       <c r="G133" s="3" t="s">
-        <v>151</v>
-      </c>
-      <c r="H133" s="3" t="s">
-        <v>147</v>
-      </c>
-      <c r="I133" s="8">
-        <v>29</v>
-      </c>
-      <c r="J133" s="8">
+        <v>155</v>
+      </c>
+      <c r="H133" s="5">
+        <v>45809</v>
+      </c>
+      <c r="I133" s="7">
+        <v>4</v>
+      </c>
+      <c r="J133" s="7">
         <v>6</v>
       </c>
     </row>
     <row r="134" spans="6:10" x14ac:dyDescent="0.25">
       <c r="F134" s="9">
-        <v>23</v>
+        <v>2</v>
       </c>
       <c r="G134" s="3" t="s">
-        <v>139</v>
-      </c>
-      <c r="H134" s="3" t="s">
-        <v>138</v>
-      </c>
-      <c r="I134" s="8">
-        <v>3</v>
-      </c>
-      <c r="J134" s="8">
-        <v>1</v>
+        <v>156</v>
+      </c>
+      <c r="H134" s="5">
+        <v>45809</v>
+      </c>
+      <c r="I134" s="7">
+        <v>4</v>
+      </c>
+      <c r="J134" s="7">
+        <v>29</v>
       </c>
     </row>
     <row r="135" spans="6:10" x14ac:dyDescent="0.25">
       <c r="F135" s="9">
-        <v>24</v>
+        <v>3</v>
       </c>
       <c r="G135" s="3" t="s">
-        <v>160</v>
-      </c>
-      <c r="H135" s="3" t="s">
-        <v>138</v>
-      </c>
-      <c r="I135" s="8">
-        <v>23</v>
-      </c>
-      <c r="J135" s="8">
-        <v>7</v>
+        <v>155</v>
+      </c>
+      <c r="H135" s="5">
+        <v>45810</v>
+      </c>
+      <c r="I135" s="7">
+        <v>2</v>
+      </c>
+      <c r="J135" s="7">
+        <v>1</v>
       </c>
     </row>
     <row r="136" spans="6:10" x14ac:dyDescent="0.25">
       <c r="F136" s="9">
-        <v>25</v>
+        <v>4</v>
       </c>
       <c r="G136" s="3" t="s">
-        <v>146</v>
-      </c>
-      <c r="H136" s="3" t="s">
-        <v>138</v>
-      </c>
-      <c r="I136" s="8">
-        <v>11</v>
-      </c>
-      <c r="J136" s="8">
-        <v>7</v>
+        <v>156</v>
+      </c>
+      <c r="H136" s="5">
+        <v>45810</v>
+      </c>
+      <c r="I136" s="7">
+        <v>3</v>
+      </c>
+      <c r="J136" s="7">
+        <v>1</v>
       </c>
     </row>
     <row r="137" spans="6:10" x14ac:dyDescent="0.25">
       <c r="F137" s="9">
-        <v>26</v>
+        <v>5</v>
       </c>
       <c r="G137" s="3" t="s">
-        <v>148</v>
-      </c>
-      <c r="H137" s="3" t="s">
-        <v>138</v>
-      </c>
-      <c r="I137" s="8">
+        <v>155</v>
+      </c>
+      <c r="H137" s="5">
+        <v>45810</v>
+      </c>
+      <c r="I137" s="7">
+        <v>5</v>
+      </c>
+      <c r="J137" s="7">
         <v>7</v>
-      </c>
-      <c r="J137" s="8">
-        <v>3</v>
       </c>
     </row>
     <row r="138" spans="6:10" x14ac:dyDescent="0.25">
       <c r="F138" s="9">
-        <v>27</v>
+        <v>6</v>
       </c>
       <c r="G138" s="3" t="s">
-        <v>143</v>
-      </c>
-      <c r="H138" s="3" t="s">
-        <v>138</v>
-      </c>
-      <c r="I138" s="8">
-        <v>1</v>
-      </c>
-      <c r="J138" s="8">
-        <v>2</v>
+        <v>155</v>
+      </c>
+      <c r="H138" s="5">
+        <v>45811</v>
+      </c>
+      <c r="I138" s="7">
+        <v>8</v>
+      </c>
+      <c r="J138" s="7">
+        <v>49</v>
       </c>
     </row>
     <row r="139" spans="6:10" x14ac:dyDescent="0.25">
       <c r="F139" s="9">
-        <v>28</v>
+        <v>7</v>
       </c>
       <c r="G139" s="3" t="s">
-        <v>143</v>
-      </c>
-      <c r="H139" s="3" t="s">
-        <v>147</v>
-      </c>
-      <c r="I139" s="8">
-        <v>1</v>
-      </c>
-      <c r="J139" s="8">
+        <v>156</v>
+      </c>
+      <c r="H139" s="5">
+        <v>45811</v>
+      </c>
+      <c r="I139" s="7">
         <v>8</v>
+      </c>
+      <c r="J139" s="7">
+        <v>60</v>
       </c>
     </row>
     <row r="140" spans="6:10" x14ac:dyDescent="0.25">
       <c r="F140" s="9">
-        <v>29</v>
+        <v>8</v>
       </c>
       <c r="G140" s="3" t="s">
-        <v>140</v>
-      </c>
-      <c r="H140" s="3" t="s">
-        <v>138</v>
-      </c>
-      <c r="I140" s="8">
-        <v>4</v>
-      </c>
-      <c r="J140" s="8">
+        <v>155</v>
+      </c>
+      <c r="H140" s="5">
+        <v>45812</v>
+      </c>
+      <c r="I140" s="7">
+        <v>6</v>
+      </c>
+      <c r="J140" s="7">
         <v>2</v>
       </c>
     </row>
     <row r="141" spans="6:10" x14ac:dyDescent="0.25">
       <c r="F141" s="9">
-        <v>30</v>
+        <v>9</v>
       </c>
       <c r="G141" s="3" t="s">
-        <v>145</v>
-      </c>
-      <c r="H141" s="3" t="s">
-        <v>138</v>
-      </c>
-      <c r="I141" s="8">
-        <v>9</v>
-      </c>
-      <c r="J141" s="8">
-        <v>3</v>
+        <v>156</v>
+      </c>
+      <c r="H141" s="5">
+        <v>45812</v>
+      </c>
+      <c r="I141" s="7">
+        <v>8</v>
+      </c>
+      <c r="J141" s="7">
+        <v>24</v>
       </c>
     </row>
     <row r="142" spans="6:10" x14ac:dyDescent="0.25">
       <c r="F142" s="9">
-        <v>31</v>
+        <v>10</v>
       </c>
       <c r="G142" s="3" t="s">
-        <v>154</v>
-      </c>
-      <c r="H142" s="3" t="s">
-        <v>147</v>
-      </c>
-      <c r="I142" s="8">
-        <v>33</v>
-      </c>
-      <c r="J142" s="8">
-        <v>5</v>
+        <v>155</v>
+      </c>
+      <c r="H142" s="5">
+        <v>45813</v>
+      </c>
+      <c r="I142" s="7">
+        <v>4</v>
+      </c>
+      <c r="J142" s="7">
+        <v>11</v>
       </c>
     </row>
     <row r="143" spans="6:10" x14ac:dyDescent="0.25">
       <c r="F143" s="9">
-        <v>32</v>
+        <v>11</v>
       </c>
       <c r="G143" s="3" t="s">
-        <v>137</v>
-      </c>
-      <c r="H143" s="3" t="s">
-        <v>138</v>
-      </c>
-      <c r="I143" s="8">
+        <v>156</v>
+      </c>
+      <c r="H143" s="5">
+        <v>45813</v>
+      </c>
+      <c r="I143" s="7">
         <v>2</v>
       </c>
-      <c r="J143" s="8">
-        <v>3</v>
+      <c r="J143" s="7">
+        <v>9</v>
       </c>
     </row>
     <row r="144" spans="6:10" x14ac:dyDescent="0.25">
       <c r="F144" s="9">
-        <v>33</v>
+        <v>12</v>
       </c>
       <c r="G144" s="3" t="s">
-        <v>142</v>
-      </c>
-      <c r="H144" s="3" t="s">
-        <v>138</v>
-      </c>
-      <c r="I144" s="8">
-        <v>6</v>
-      </c>
-      <c r="J144" s="8">
+        <v>155</v>
+      </c>
+      <c r="H144" s="5">
+        <v>45813</v>
+      </c>
+      <c r="I144" s="7">
         <v>1</v>
+      </c>
+      <c r="J144" s="7">
+        <v>5</v>
       </c>
     </row>
     <row r="145" spans="6:10" x14ac:dyDescent="0.25">
       <c r="F145" s="9">
-        <v>34</v>
+        <v>13</v>
       </c>
       <c r="G145" s="3" t="s">
-        <v>148</v>
-      </c>
-      <c r="H145" s="3" t="s">
-        <v>138</v>
-      </c>
-      <c r="I145" s="8">
-        <v>7</v>
-      </c>
-      <c r="J145" s="8">
-        <v>1</v>
+        <v>156</v>
+      </c>
+      <c r="H145" s="5">
+        <v>45814</v>
+      </c>
+      <c r="I145" s="7">
+        <v>8</v>
+      </c>
+      <c r="J145" s="7">
+        <v>33</v>
       </c>
     </row>
     <row r="146" spans="6:10" x14ac:dyDescent="0.25">
       <c r="F146" s="9">
-        <v>35</v>
+        <v>14</v>
       </c>
       <c r="G146" s="3" t="s">
         <v>155</v>
       </c>
-      <c r="H146" s="3" t="s">
-        <v>138</v>
-      </c>
-      <c r="I146" s="8">
-        <v>22</v>
-      </c>
-      <c r="J146" s="8">
-        <v>5</v>
+      <c r="H146" s="5">
+        <v>45814</v>
+      </c>
+      <c r="I146" s="7">
+        <v>4</v>
+      </c>
+      <c r="J146" s="7">
+        <v>1</v>
       </c>
     </row>
     <row r="147" spans="6:10" x14ac:dyDescent="0.25">
       <c r="F147" s="9">
-        <v>36</v>
+        <v>15</v>
       </c>
       <c r="G147" s="3" t="s">
-        <v>166</v>
-      </c>
-      <c r="H147" s="3" t="s">
-        <v>138</v>
-      </c>
-      <c r="I147" s="8">
+        <v>156</v>
+      </c>
+      <c r="H147" s="5">
+        <v>45815</v>
+      </c>
+      <c r="I147" s="7">
+        <v>8</v>
+      </c>
+      <c r="J147" s="7">
         <v>12</v>
       </c>
-      <c r="J147" s="8">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="148" spans="6:10" x14ac:dyDescent="0.25">
-      <c r="F148" s="9">
-        <v>37</v>
-      </c>
-      <c r="G148" s="3" t="s">
-        <v>156</v>
-      </c>
-      <c r="H148" s="3" t="s">
-        <v>138</v>
-      </c>
-      <c r="I148" s="8">
-        <v>32</v>
-      </c>
-      <c r="J148" s="8">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="149" spans="6:10" x14ac:dyDescent="0.25">
-      <c r="F149" s="9">
-        <v>38</v>
-      </c>
-      <c r="G149" s="3" t="s">
-        <v>157</v>
-      </c>
-      <c r="H149" s="3" t="s">
-        <v>138</v>
-      </c>
-      <c r="I149" s="8">
-        <v>14</v>
-      </c>
-      <c r="J149" s="8">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="150" spans="6:10" x14ac:dyDescent="0.25">
-      <c r="F150" s="9">
-        <v>39</v>
-      </c>
-      <c r="G150" s="3" t="s">
-        <v>146</v>
-      </c>
-      <c r="H150" s="3" t="s">
-        <v>147</v>
-      </c>
-      <c r="I150" s="8">
-        <v>11</v>
-      </c>
-      <c r="J150" s="8">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="151" spans="6:10" x14ac:dyDescent="0.25">
-      <c r="F151" s="9">
-        <v>40</v>
-      </c>
-      <c r="G151" s="3" t="s">
-        <v>167</v>
-      </c>
-      <c r="H151" s="3" t="s">
-        <v>138</v>
-      </c>
-      <c r="I151" s="8">
-        <v>25</v>
-      </c>
-      <c r="J151" s="8">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="155" spans="6:10" x14ac:dyDescent="0.25">
-      <c r="F155" s="11" t="s">
-        <v>206</v>
-      </c>
-      <c r="G155" s="11"/>
-      <c r="H155" s="11"/>
-      <c r="I155" s="11"/>
-      <c r="J155" s="11"/>
-    </row>
-    <row r="156" spans="6:10" x14ac:dyDescent="0.25">
-      <c r="F156" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="G156" s="2" t="s">
-        <v>136</v>
-      </c>
-      <c r="H156" s="2" t="s">
-        <v>168</v>
-      </c>
-      <c r="I156" s="2" t="s">
-        <v>173</v>
-      </c>
-      <c r="J156" s="2" t="s">
-        <v>174</v>
-      </c>
-    </row>
-    <row r="157" spans="6:10" x14ac:dyDescent="0.25">
-      <c r="F157" s="10">
-        <v>1</v>
-      </c>
-      <c r="G157" s="3" t="s">
-        <v>171</v>
-      </c>
-      <c r="H157" s="6">
-        <v>45809.375</v>
-      </c>
-      <c r="I157" s="8">
-        <v>2</v>
-      </c>
-      <c r="J157" s="8">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="158" spans="6:10" x14ac:dyDescent="0.25">
-      <c r="F158" s="10">
-        <v>2</v>
-      </c>
-      <c r="G158" s="3" t="s">
-        <v>172</v>
-      </c>
-      <c r="H158" s="6">
-        <v>45809.381944444445</v>
-      </c>
-      <c r="I158" s="8">
-        <v>9</v>
-      </c>
-      <c r="J158" s="8">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="159" spans="6:10" x14ac:dyDescent="0.25">
-      <c r="F159" s="10">
-        <v>3</v>
-      </c>
-      <c r="G159" s="3" t="s">
-        <v>171</v>
-      </c>
-      <c r="H159" s="6">
-        <v>45809.388888888891</v>
-      </c>
-      <c r="I159" s="8">
-        <v>3</v>
-      </c>
-      <c r="J159" s="8">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="160" spans="6:10" x14ac:dyDescent="0.25">
-      <c r="F160" s="10">
-        <v>4</v>
-      </c>
-      <c r="G160" s="3" t="s">
-        <v>172</v>
-      </c>
-      <c r="H160" s="6">
-        <v>45809.416666666664</v>
-      </c>
-      <c r="I160" s="8">
-        <v>14</v>
-      </c>
-      <c r="J160" s="8">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="161" spans="6:10" x14ac:dyDescent="0.25">
-      <c r="F161" s="10">
-        <v>5</v>
-      </c>
-      <c r="G161" s="3" t="s">
-        <v>171</v>
-      </c>
-      <c r="H161" s="6">
-        <v>45809.458333333336</v>
-      </c>
-      <c r="I161" s="8">
-        <v>1</v>
-      </c>
-      <c r="J161" s="8">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="162" spans="6:10" x14ac:dyDescent="0.25">
-      <c r="F162" s="10">
-        <v>6</v>
-      </c>
-      <c r="G162" s="3" t="s">
-        <v>171</v>
-      </c>
-      <c r="H162" s="6">
-        <v>45809.479166666664</v>
-      </c>
-      <c r="I162" s="8">
-        <v>4</v>
-      </c>
-      <c r="J162" s="8">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="163" spans="6:10" x14ac:dyDescent="0.25">
-      <c r="F163" s="10">
-        <v>7</v>
-      </c>
-      <c r="G163" s="3" t="s">
-        <v>172</v>
-      </c>
-      <c r="H163" s="6">
-        <v>45810.364583333336</v>
-      </c>
-      <c r="I163" s="8">
-        <v>8</v>
-      </c>
-      <c r="J163" s="8">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="164" spans="6:10" x14ac:dyDescent="0.25">
-      <c r="F164" s="10">
-        <v>8</v>
-      </c>
-      <c r="G164" s="3" t="s">
-        <v>171</v>
-      </c>
-      <c r="H164" s="6">
-        <v>45810.375</v>
-      </c>
-      <c r="I164" s="8">
-        <v>7</v>
-      </c>
-      <c r="J164" s="8">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="165" spans="6:10" x14ac:dyDescent="0.25">
-      <c r="F165" s="10">
-        <v>9</v>
-      </c>
-      <c r="G165" s="3" t="s">
-        <v>172</v>
-      </c>
-      <c r="H165" s="6">
-        <v>45810.395833333336</v>
-      </c>
-      <c r="I165" s="8">
-        <v>16</v>
-      </c>
-      <c r="J165" s="8">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="166" spans="6:10" x14ac:dyDescent="0.25">
-      <c r="F166" s="10">
-        <v>10</v>
-      </c>
-      <c r="G166" s="3" t="s">
-        <v>171</v>
-      </c>
-      <c r="H166" s="6">
-        <v>45810.427083333336</v>
-      </c>
-      <c r="I166" s="8">
-        <v>10</v>
-      </c>
-      <c r="J166" s="8">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="167" spans="6:10" x14ac:dyDescent="0.25">
-      <c r="F167" s="10">
-        <v>11</v>
-      </c>
-      <c r="G167" s="3" t="s">
-        <v>172</v>
-      </c>
-      <c r="H167" s="6">
-        <v>45811.583333333336</v>
-      </c>
-      <c r="I167" s="8">
-        <v>18</v>
-      </c>
-      <c r="J167" s="8">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="168" spans="6:10" x14ac:dyDescent="0.25">
-      <c r="F168" s="10">
-        <v>12</v>
-      </c>
-      <c r="G168" s="3" t="s">
-        <v>171</v>
-      </c>
-      <c r="H168" s="6">
-        <v>45811.604166666664</v>
-      </c>
-      <c r="I168" s="8">
-        <v>27</v>
-      </c>
-      <c r="J168" s="8">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="169" spans="6:10" x14ac:dyDescent="0.25">
-      <c r="F169" s="10">
-        <v>13</v>
-      </c>
-      <c r="G169" s="3" t="s">
-        <v>171</v>
-      </c>
-      <c r="H169" s="6">
-        <v>45811.635416666664</v>
-      </c>
-      <c r="I169" s="8">
-        <v>5</v>
-      </c>
-      <c r="J169" s="8">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="170" spans="6:10" x14ac:dyDescent="0.25">
-      <c r="F170" s="10">
-        <v>14</v>
-      </c>
-      <c r="G170" s="3" t="s">
-        <v>172</v>
-      </c>
-      <c r="H170" s="6">
-        <v>45811.666666666664</v>
-      </c>
-      <c r="I170" s="8">
-        <v>24</v>
-      </c>
-      <c r="J170" s="8">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="171" spans="6:10" x14ac:dyDescent="0.25">
-      <c r="F171" s="10">
-        <v>15</v>
-      </c>
-      <c r="G171" s="3" t="s">
-        <v>171</v>
-      </c>
-      <c r="H171" s="6">
-        <v>45812.388888888891</v>
-      </c>
-      <c r="I171" s="8">
-        <v>22</v>
-      </c>
-      <c r="J171" s="8">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="172" spans="6:10" x14ac:dyDescent="0.25">
-      <c r="F172" s="10">
-        <v>16</v>
-      </c>
-      <c r="G172" s="3" t="s">
-        <v>172</v>
-      </c>
-      <c r="H172" s="6">
-        <v>45812.416666666664</v>
-      </c>
-      <c r="I172" s="8">
-        <v>13</v>
-      </c>
-      <c r="J172" s="8">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="173" spans="6:10" x14ac:dyDescent="0.25">
-      <c r="F173" s="10">
-        <v>17</v>
-      </c>
-      <c r="G173" s="3" t="s">
-        <v>171</v>
-      </c>
-      <c r="H173" s="6">
-        <v>45812.4375</v>
-      </c>
-      <c r="I173" s="8">
-        <v>7</v>
-      </c>
-      <c r="J173" s="8">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="174" spans="6:10" x14ac:dyDescent="0.25">
-      <c r="F174" s="10">
-        <v>18</v>
-      </c>
-      <c r="G174" s="3" t="s">
-        <v>172</v>
-      </c>
-      <c r="H174" s="6">
-        <v>45812.458333333336</v>
-      </c>
-      <c r="I174" s="8">
-        <v>28</v>
-      </c>
-      <c r="J174" s="8">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="175" spans="6:10" x14ac:dyDescent="0.25">
-      <c r="F175" s="10">
-        <v>19</v>
-      </c>
-      <c r="G175" s="3" t="s">
-        <v>171</v>
-      </c>
-      <c r="H175" s="6">
-        <v>45813.541666666664</v>
-      </c>
-      <c r="I175" s="8">
-        <v>6</v>
-      </c>
-      <c r="J175" s="8">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="176" spans="6:10" x14ac:dyDescent="0.25">
-      <c r="F176" s="10">
-        <v>20</v>
-      </c>
-      <c r="G176" s="3" t="s">
-        <v>171</v>
-      </c>
-      <c r="H176" s="6">
-        <v>45813.572916666664</v>
-      </c>
-      <c r="I176" s="8">
-        <v>32</v>
-      </c>
-      <c r="J176" s="8">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="177" spans="6:10" x14ac:dyDescent="0.25">
-      <c r="F177" s="10">
-        <v>21</v>
-      </c>
-      <c r="G177" s="3" t="s">
-        <v>172</v>
-      </c>
-      <c r="H177" s="6">
-        <v>45813.604166666664</v>
-      </c>
-      <c r="I177" s="8">
-        <v>21</v>
-      </c>
-      <c r="J177" s="8">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="178" spans="6:10" x14ac:dyDescent="0.25">
-      <c r="F178" s="10">
-        <v>22</v>
-      </c>
-      <c r="G178" s="3" t="s">
-        <v>171</v>
-      </c>
-      <c r="H178" s="6">
-        <v>45813.635416666664</v>
-      </c>
-      <c r="I178" s="8">
-        <v>9</v>
-      </c>
-      <c r="J178" s="8">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="179" spans="6:10" x14ac:dyDescent="0.25">
-      <c r="F179" s="10">
-        <v>23</v>
-      </c>
-      <c r="G179" s="3" t="s">
-        <v>172</v>
-      </c>
-      <c r="H179" s="6">
-        <v>45813.652777777781</v>
-      </c>
-      <c r="I179" s="8">
-        <v>31</v>
-      </c>
-      <c r="J179" s="8">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="180" spans="6:10" x14ac:dyDescent="0.25">
-      <c r="F180" s="10">
-        <v>24</v>
-      </c>
-      <c r="G180" s="3" t="s">
-        <v>171</v>
-      </c>
-      <c r="H180" s="6">
-        <v>45813.673611111109</v>
-      </c>
-      <c r="I180" s="8">
-        <v>29</v>
-      </c>
-      <c r="J180" s="8">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="181" spans="6:10" x14ac:dyDescent="0.25">
-      <c r="F181" s="10">
-        <v>25</v>
-      </c>
-      <c r="G181" s="3" t="s">
-        <v>172</v>
-      </c>
-      <c r="H181" s="6">
-        <v>45813.708333333336</v>
-      </c>
-      <c r="I181" s="8">
-        <v>17</v>
-      </c>
-      <c r="J181" s="8">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="182" spans="6:10" x14ac:dyDescent="0.25">
-      <c r="F182" s="10">
-        <v>26</v>
-      </c>
-      <c r="G182" s="3" t="s">
-        <v>171</v>
-      </c>
-      <c r="H182" s="6">
-        <v>45813.729166666664</v>
-      </c>
-      <c r="I182" s="8">
-        <v>39</v>
-      </c>
-      <c r="J182" s="8">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="183" spans="6:10" x14ac:dyDescent="0.25">
-      <c r="F183" s="10">
-        <v>27</v>
-      </c>
-      <c r="G183" s="3" t="s">
-        <v>171</v>
-      </c>
-      <c r="H183" s="6">
-        <v>45814.395833333336</v>
-      </c>
-      <c r="I183" s="8">
-        <v>1</v>
-      </c>
-      <c r="J183" s="8">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="184" spans="6:10" x14ac:dyDescent="0.25">
-      <c r="F184" s="10">
-        <v>28</v>
-      </c>
-      <c r="G184" s="3" t="s">
-        <v>171</v>
-      </c>
-      <c r="H184" s="6">
-        <v>45814.416666666664</v>
-      </c>
-      <c r="I184" s="8">
-        <v>13</v>
-      </c>
-      <c r="J184" s="8">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="185" spans="6:10" x14ac:dyDescent="0.25">
-      <c r="F185" s="10">
-        <v>29</v>
-      </c>
-      <c r="G185" s="3" t="s">
-        <v>172</v>
-      </c>
-      <c r="H185" s="6">
-        <v>45814.458333333336</v>
-      </c>
-      <c r="I185" s="8">
-        <v>23</v>
-      </c>
-      <c r="J185" s="8">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="186" spans="6:10" x14ac:dyDescent="0.25">
-      <c r="F186" s="10">
-        <v>30</v>
-      </c>
-      <c r="G186" s="3" t="s">
-        <v>171</v>
-      </c>
-      <c r="H186" s="6">
-        <v>45815.354166666664</v>
-      </c>
-      <c r="I186" s="8">
-        <v>2</v>
-      </c>
-      <c r="J186" s="8">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="187" spans="6:10" x14ac:dyDescent="0.25">
-      <c r="F187" s="10">
-        <v>31</v>
-      </c>
-      <c r="G187" s="3" t="s">
-        <v>171</v>
-      </c>
-      <c r="H187" s="6">
-        <v>45815.385416666664</v>
-      </c>
-      <c r="I187" s="8">
-        <v>27</v>
-      </c>
-      <c r="J187" s="8">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="188" spans="6:10" x14ac:dyDescent="0.25">
-      <c r="F188" s="10">
-        <v>32</v>
-      </c>
-      <c r="G188" s="3" t="s">
-        <v>172</v>
-      </c>
-      <c r="H188" s="6">
-        <v>45815.40625</v>
-      </c>
-      <c r="I188" s="8">
-        <v>37</v>
-      </c>
-      <c r="J188" s="8">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="189" spans="6:10" x14ac:dyDescent="0.25">
-      <c r="F189" s="10">
-        <v>33</v>
-      </c>
-      <c r="G189" s="3" t="s">
-        <v>171</v>
-      </c>
-      <c r="H189" s="6">
-        <v>45816.416666666664</v>
-      </c>
-      <c r="I189" s="8">
-        <v>5</v>
-      </c>
-      <c r="J189" s="8">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="190" spans="6:10" x14ac:dyDescent="0.25">
-      <c r="F190" s="10">
-        <v>34</v>
-      </c>
-      <c r="G190" s="3" t="s">
-        <v>172</v>
-      </c>
-      <c r="H190" s="6">
-        <v>45816.458333333336</v>
-      </c>
-      <c r="I190" s="8">
-        <v>33</v>
-      </c>
-      <c r="J190" s="8">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="191" spans="6:10" x14ac:dyDescent="0.25">
-      <c r="F191" s="10">
-        <v>35</v>
-      </c>
-      <c r="G191" s="3" t="s">
-        <v>171</v>
-      </c>
-      <c r="H191" s="6">
-        <v>45816.5</v>
-      </c>
-      <c r="I191" s="8">
-        <v>11</v>
-      </c>
-      <c r="J191" s="8">
-        <v>12</v>
-      </c>
     </row>
   </sheetData>
-  <mergeCells count="4">
-    <mergeCell ref="F155:J155"/>
-    <mergeCell ref="F3:G3"/>
+  <mergeCells count="3">
+    <mergeCell ref="F131:J131"/>
     <mergeCell ref="D36:K36"/>
     <mergeCell ref="F110:J110"/>
   </mergeCells>
@@ -4723,15 +3692,15 @@
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6C0FA18E-0926-46C2-B252-4A5E541FB5A0}">
   <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="87289aac-3191-415d-94b6-004c2ae78a31"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
     <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
     <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="87289aac-3191-415d-94b6-004c2ae78a31"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>